<commit_message>
updated bento multifilter test scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Canine_E2E_MultipleFilters-Study_Breed_Sex.xlsx
+++ b/InputFiles/TC03_Canine_E2E_MultipleFilters-Study_Breed_Sex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F678DEA-5748-47D3-BF6D-A673199A70DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2252215-6D87-433A-ADD5-9AD9B1F5FA4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>WebExcel</t>
   </si>
@@ -43,12 +43,6 @@
     <t>dbExcel</t>
   </si>
   <si>
-    <t>TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_Canine_Filter_Breed-Akita_WebData.xlsx</t>
-  </si>
-  <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
   <si>
@@ -59,46 +53,6 @@
   </si>
   <si>
     <t>CasesTab</t>
-  </si>
-  <si>
-    <t>SamplesTab</t>
-  </si>
-  <si>
-    <t>FilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE demo.breed IN ['Akita']  
-OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN  coalesce(f.file_name, '') AS `File Name`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE demo.breed IN ['Akita'] 
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed,
-        coalesce(diag.disease_term,'') AS Diagnosis, 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
     <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -126,6 +80,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>TC03_Canine_E2E_MultipleFilters-Study_Breed_Sex_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC03_Canine_E2E_MultipleFilters-Study_Breed_Sex_WebData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -496,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,13 +473,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -528,68 +488,34 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C5" s="1"/>
@@ -611,12 +537,6 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>